<commit_message>
Updated things. Late nights, too much weed
</commit_message>
<xml_diff>
--- a/Script Printer.xlsx
+++ b/Script Printer.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cryptopoly/CryptopoTools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6221DB05-A828-174E-82AA-C8C6F88CAC58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B1ED97A-E0F9-C64A-82D0-B653CF3035A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="6560" windowWidth="28040" windowHeight="17440" xr2:uid="{268F1EFA-AF22-BE47-9497-01FDDA25BD0D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" xr2:uid="{268F1EFA-AF22-BE47-9497-01FDDA25BD0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Troubleshooting" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
-  <si>
-    <t>#Ocean</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>cd $HOME</t>
   </si>
@@ -99,24 +96,12 @@
     <t>make -j4</t>
   </si>
   <si>
-    <t>#Dependencies</t>
-  </si>
-  <si>
     <t>git clone https://github.com/goldtokensa/dependencies.git</t>
   </si>
   <si>
     <t>cd $HOME/dependencies</t>
   </si>
   <si>
-    <t>pip3 install -r boto3/requirements.txt</t>
-  </si>
-  <si>
-    <t>pip3 install -e boto3 -e python-mnemonic -e datadiff-2.0.0 -e pybitcointools -e requests</t>
-  </si>
-  <si>
-    <t>#Asset Mapping</t>
-  </si>
-  <si>
     <t>git clone https://github.com/commerceblock/asset-mapping.git</t>
   </si>
   <si>
@@ -141,24 +126,12 @@
     <t>chmod +x *.py</t>
   </si>
   <si>
-    <t>gsettings set org.gnome.nautilus.preferences executable-text-activation launch</t>
-  </si>
-  <si>
-    <t>ln -s /home/dgld-v2/asset-mapping/macos-scripts/DGLD_Command_Centre.command $HOME/Desktop</t>
-  </si>
-  <si>
-    <t>#CB Electrum Wallet</t>
-  </si>
-  <si>
     <t>git clone https://github.com/commerceblock/cb-client-wallet.git</t>
   </si>
   <si>
     <t>cd $HOME/cb-client-wallet</t>
   </si>
   <si>
-    <t>sudo apt install pyqt5-dev-tools</t>
-  </si>
-  <si>
     <t>pyrcc5 icons.qrc -o electrum/gui/qt/icons_rc.py</t>
   </si>
   <si>
@@ -168,9 +141,6 @@
     <t>Code</t>
   </si>
   <si>
-    <t>pip3 install .[fast] -y</t>
-  </si>
-  <si>
     <t>./electrum-env</t>
   </si>
   <si>
@@ -178,6 +148,48 @@
   </si>
   <si>
     <t xml:space="preserve">Lol just use </t>
+  </si>
+  <si>
+    <t>set -x</t>
+  </si>
+  <si>
+    <t># Ocean</t>
+  </si>
+  <si>
+    <t># Dependencies</t>
+  </si>
+  <si>
+    <t># Asset Mapping</t>
+  </si>
+  <si>
+    <t># CB Electrum Wallet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sudo apt install pyqt5-dev-tools -y </t>
+  </si>
+  <si>
+    <t># Log</t>
+  </si>
+  <si>
+    <t>gsettings set org.gnome.nautilus.preferences executable-text-activation ask</t>
+  </si>
+  <si>
+    <t>sudo apt install curl -y</t>
+  </si>
+  <si>
+    <t>mkdir goldnode_main</t>
+  </si>
+  <si>
+    <t>sudo pip3 install -r boto3/requirements.txt</t>
+  </si>
+  <si>
+    <t>sudo pip3 install -e boto3 -e python-mnemonic -e datadiff-2.0.0 -e pybitcointools -e requests</t>
+  </si>
+  <si>
+    <t>sudo ln -s /home/dgld-v2/asset-mapping/macos-scripts/DGLD_Command_Centre.command $HOME/Desktop</t>
+  </si>
+  <si>
+    <t>sudo pip3 install .[fast]</t>
   </si>
 </sst>
 </file>
@@ -261,8 +273,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{90DC9FE6-3B42-7F4B-BC24-4BF3B3BF09CD}" name="Table2" displayName="Table2" ref="B4:C54" totalsRowShown="0">
-  <autoFilter ref="B4:C54" xr:uid="{B349DA02-6DC7-4C4F-B24C-B67555877034}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{90DC9FE6-3B42-7F4B-BC24-4BF3B3BF09CD}" name="Table2" displayName="Table2" ref="B4:C58" totalsRowShown="0">
+  <autoFilter ref="B4:C58" xr:uid="{B349DA02-6DC7-4C4F-B24C-B67555877034}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{CC32FCD5-B64F-1C47-B3E0-5CE677AB0C3C}" name="Command"/>
     <tableColumn id="2" xr3:uid="{C5434F8D-DB2F-4246-A171-53D0130BC2D7}" name="Code" dataDxfId="0">
@@ -570,10 +582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6066F9D8-A3BE-6C4F-83E8-A638A1931F7D}">
-  <dimension ref="B2:C54"/>
+  <dimension ref="B2:C58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5:C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -584,463 +596,499 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="C5" s="3" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: #Ocean"</v>
+        <v>; pwd ; echo "Bash: # Log"</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B6" s="2" t="s">
-        <v>1</v>
+      <c r="B6" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="C6" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: cd $HOME"</v>
+        <v>; pwd ; echo "Bash: set -x"</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B7" s="2" t="s">
-        <v>2</v>
+      <c r="B7" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="C7" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: sudo apt install git -y"</v>
+        <v>; pwd ; echo "Bash: # Ocean"</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C8" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: git clone https://github.com/commerceblock/ocean"</v>
+        <v>; pwd ; echo "Bash: cd $HOME"</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="s">
-        <v>4</v>
+      <c r="B9" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="C9" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: cd $HOME/ocean"</v>
+        <v>; pwd ; echo "Bash: sudo apt install git -y"</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="C10" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: sudo add-apt-repository ppa:bitcoin/bitcoin -y"</v>
+        <v>; pwd ; echo "Bash: sudo apt install curl -y"</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C11" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: sudo apt update -y"</v>
+        <v>; pwd ; echo "Bash: git clone https://github.com/commerceblock/ocean"</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B12" s="2" t="s">
-        <v>7</v>
+      <c r="B12" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="C12" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: sudo apt dist-upgrade -y"</v>
+        <v>; pwd ; echo "Bash: cd $HOME/ocean"</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C13" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: sudo apt install autoconf -y"</v>
+        <v>; pwd ; echo "Bash: sudo add-apt-repository ppa:bitcoin/bitcoin -y"</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C14" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: sudo apt install libtool -y"</v>
+        <v>; pwd ; echo "Bash: sudo apt update -y"</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C15" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: sudo apt install pkg-config -y"</v>
+        <v>; pwd ; echo "Bash: sudo apt dist-upgrade -y"</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C16" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: sudo apt install libboost-all-dev -y"</v>
+        <v>; pwd ; echo "Bash: sudo apt install autoconf -y"</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C17" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: sudo apt install libdb4.8-dev libdb4.8++-dev -y "</v>
+        <v>; pwd ; echo "Bash: sudo apt install libtool -y"</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C18" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: sudo apt install -dist openssl -y"</v>
+        <v>; pwd ; echo "Bash: sudo apt install pkg-config -y"</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C19" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: sudo apt install libssl-dev -y"</v>
+        <v>; pwd ; echo "Bash: sudo apt install libboost-all-dev -y"</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C20" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: sudo apt install libevent-dev -y"</v>
+        <v>; pwd ; echo "Bash: sudo apt install libdb4.8-dev libdb4.8++-dev -y "</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C21" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: sudo apt install python3-pip -y"</v>
+        <v>; pwd ; echo "Bash: sudo apt install -dist openssl -y"</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C22" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
+        <v>; pwd ; echo "Bash: sudo apt install libssl-dev -y"</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" t="str">
+        <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
+        <v>; pwd ; echo "Bash: sudo apt install libevent-dev -y"</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" t="str">
+        <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
+        <v>; pwd ; echo "Bash: sudo apt install python3-pip -y"</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" t="str">
+        <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
         <v>; pwd ; echo "Bash: sudo apt autoremove -y"</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B23" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" t="str">
-        <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: ./autogen.sh"</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B24" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C24" t="str">
-        <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: ./configure"</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B25" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C25" t="str">
-        <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: make"</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C26" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: make -j4"</v>
+        <v>; pwd ; echo "Bash: ./autogen.sh"</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B27" s="2" t="s">
-        <v>1</v>
+      <c r="B27" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="C27" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: cd $HOME"</v>
+        <v>; pwd ; echo "Bash: ./configure"</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C28" s="3" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: #Dependencies"</v>
+        <v>; pwd ; echo "Bash: make"</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C29" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
+        <v>; pwd ; echo "Bash: make -j4"</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B30" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" t="str">
+        <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
         <v>; pwd ; echo "Bash: cd $HOME"</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B30" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C30" t="str">
-        <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: git clone https://github.com/goldtokensa/dependencies.git"</v>
-      </c>
-    </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B31" s="1" t="s">
-        <v>24</v>
+      <c r="B31" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="C31" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: cd $HOME/dependencies"</v>
+        <v>; pwd ; echo "Bash: mkdir goldnode_main"</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="C32" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: pip3 install -r boto3/requirements.txt"</v>
+        <v>; pwd ; echo "Bash: # Dependencies"</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="C33" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: pip3 install -e boto3 -e python-mnemonic -e datadiff-2.0.0 -e pybitcointools -e requests"</v>
+        <v>; pwd ; echo "Bash: cd $HOME"</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C34" s="3" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: #Asset Mapping"</v>
+        <v>; pwd ; echo "Bash: git clone https://github.com/goldtokensa/dependencies.git"</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C35" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: cd $HOME"</v>
+        <v>; pwd ; echo "Bash: cd $HOME/dependencies"</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="C36" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: git clone https://github.com/commerceblock/asset-mapping.git"</v>
+        <v>; pwd ; echo "Bash: sudo pip3 install -r boto3/requirements.txt"</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="C37" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: cd $HOME/asset-mapping"</v>
+        <v>; pwd ; echo "Bash: sudo pip3 install -e boto3 -e python-mnemonic -e datadiff-2.0.0 -e pybitcointools -e requests"</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="C38" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: sudo python3 setup.py install"</v>
+        <v>; pwd ; echo "Bash: # Asset Mapping"</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="C39" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: cd $HOME/asset-mapping/macos-scripts"</v>
+        <v>; pwd ; echo "Bash: cd $HOME"</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C40" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: chmod +x *.sh"</v>
+        <v>; pwd ; echo "Bash: git clone https://github.com/commerceblock/asset-mapping.git"</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C41" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: chmod +x *.command"</v>
+        <v>; pwd ; echo "Bash: cd $HOME/asset-mapping"</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C42" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: chmod +x *.desktop"</v>
+        <v>; pwd ; echo "Bash: sudo python3 setup.py install"</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C43" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: chmod +x *.py"</v>
+        <v>; pwd ; echo "Bash: cd $HOME/asset-mapping/macos-scripts"</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C44" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: gsettings set org.gnome.nautilus.preferences executable-text-activation launch"</v>
+        <v>; pwd ; echo "Bash: chmod +x *.sh"</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C45" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: ln -s /home/dgld-v2/asset-mapping/macos-scripts/DGLD_Command_Centre.command $HOME/Desktop"</v>
+        <v>; pwd ; echo "Bash: chmod +x *.command"</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C46" s="3" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: #CB Electrum Wallet"</v>
+        <v>; pwd ; echo "Bash: chmod +x *.desktop"</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="C47" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: cd $HOME"</v>
+        <v>; pwd ; echo "Bash: chmod +x *.py"</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B48" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C48" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: git clone https://github.com/commerceblock/cb-client-wallet.git"</v>
+        <v>; pwd ; echo "Bash: gsettings set org.gnome.nautilus.preferences executable-text-activation ask"</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B49" s="1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="C49" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: cd $HOME/cb-client-wallet"</v>
+        <v>; pwd ; echo "Bash: sudo ln -s /home/dgld-v2/asset-mapping/macos-scripts/DGLD_Command_Centre.command $HOME/Desktop"</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B50" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C50" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: pip3 install .[fast] -y"</v>
+        <v>; pwd ; echo "Bash: # CB Electrum Wallet"</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B51" s="1" t="s">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="C51" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: sudo apt install pyqt5-dev-tools"</v>
+        <v>; pwd ; echo "Bash: cd $HOME"</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B52" s="1" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C52" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: pyrcc5 icons.qrc -o electrum/gui/qt/icons_rc.py"</v>
+        <v>; pwd ; echo "Bash: git clone https://github.com/commerceblock/cb-client-wallet.git"</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B53" s="1" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="C53" s="4" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
-        <v>; pwd ; echo "Bash: ./electrum-env"</v>
+        <v>; pwd ; echo "Bash: cd $HOME/cb-client-wallet"</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B54" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C54" s="4" t="str">
+        <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
+        <v>; pwd ; echo "Bash: sudo pip3 install .[fast]"</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B55" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C55" s="4" t="str">
+        <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
+        <v>; pwd ; echo "Bash: sudo apt install pyqt5-dev-tools -y "</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B56" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C56" s="4" t="str">
+        <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
+        <v>; pwd ; echo "Bash: pyrcc5 icons.qrc -o electrum/gui/qt/icons_rc.py"</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B57" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C57" s="4" t="str">
+        <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
+        <v>; pwd ; echo "Bash: ./electrum-env"</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B58" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C58" s="4" t="str">
         <f>_xlfn.CONCAT("; pwd ; echo ""Bash: ",Table2[[#This Row],[Command]],"""")</f>
         <v>; pwd ; echo "Bash: ./run_electrum"</v>
       </c>

</xml_diff>